<commit_message>
update with NE traverses
</commit_message>
<xml_diff>
--- a/planning_info/NE_2021_Aug_DD_Borek.xlsx
+++ b/planning_info/NE_2021_Aug_DD_Borek.xlsx
@@ -190,7 +190,7 @@
     <t>EGP new AWS install. Twin Otter overnights</t>
   </si>
   <si>
-    <t>maintanance at Summit</t>
+    <t>maintanance at NASA-E</t>
   </si>
   <si>
     <t>return to EGP for overnight 2</t>
@@ -202,7 +202,7 @@
     <t>return to coast. Upernavik</t>
   </si>
   <si>
-    <t>return toward Iceland</t>
+    <t>return to Canada</t>
   </si>
 </sst>
 </file>

</xml_diff>